<commit_message>
suppression page etude complementaire d7005226a0f72d78624c99894ca889b748fbd2a6
</commit_message>
<xml_diff>
--- a/FinalisationMappingPosologie/ig/PN13-FHIR-FreeSetCIODC-Unite-ConceptMap.xlsx
+++ b/FinalisationMappingPosologie/ig/PN13-FHIR-FreeSetCIODC-Unite-ConceptMap.xlsx
@@ -105,7 +105,7 @@
     <t>https://www.phast.fr/ciodm/|2025</t>
   </si>
   <si>
-    <t>https://ucum.org/</t>
+    <t>http://unitsofmeasure.org</t>
   </si>
   <si>
     <t>10*3.bq</t>
@@ -1035,7 +1035,7 @@
     <t>pst</t>
   </si>
   <si>
-    <t>bandg}</t>
+    <t>{bandg}</t>
   </si>
   <si>
     <t>pulv</t>

</xml_diff>